<commit_message>
Finished coding the stimulus presentation intervals. Now, the fixation is presented before each interval and removed during stimulus presentation.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1_train.xlsx
+++ b/cond-files/cond_pm1_train.xlsx
@@ -1,31 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\eb\eb\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1FD737-45CF-440E-93E2-F95BF088EE0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EB8998-A5D9-4045-8ED9-7212630F91D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="92" yWindow="144" windowWidth="16259" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23263" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="cond_eb1_c" sheetId="1" r:id="rId1"/>
+    <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>targ_right</t>
+    <t>stim1_c</t>
   </si>
   <si>
-    <t>cue_valid</t>
+    <t>stim2_c</t>
+  </si>
+  <si>
+    <t>SOA</t>
+  </si>
+  <si>
+    <t>angle_diff</t>
   </si>
 </sst>
 </file>
@@ -891,84 +904,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>-0.4</v>
+      </c>
+      <c r="D2">
+        <v>-0.4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
+      <c r="C3">
+        <v>-0.4</v>
+      </c>
+      <c r="D3">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaked responses and made intervals more distinct. Better print-to-screen. Coded the debug-specific timing. File output. Experimental (non-debug) mode. Included a preliminary confidence judgment.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1_train.xlsx
+++ b/cond-files/cond_pm1_train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EB8998-A5D9-4045-8ED9-7212630F91D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CA47B8-BBD4-4EC7-897B-D19F673C6A82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23263" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -904,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>-0.4</v>
@@ -945,13 +945,69 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>-0.4</v>
       </c>
       <c r="D3">
         <v>-0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-0.4</v>
+      </c>
+      <c r="D4">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>-0.4</v>
+      </c>
+      <c r="D5">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>-1.6</v>
+      </c>
+      <c r="D6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>-1.6</v>
+      </c>
+      <c r="D7">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bunch of bugs and started on the analysis.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1_train.xlsx
+++ b/cond-files/cond_pm1_train.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CA47B8-BBD4-4EC7-897B-D19F673C6A82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B86DD2-AE48-4501-8C8E-F9E93D2EBAB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23263" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-144" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
@@ -904,13 +904,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B8" sqref="B8:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>-0.4</v>
+        <v>-2</v>
       </c>
       <c r="D4">
         <v>-2</v>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>-0.4</v>
+        <v>-2</v>
       </c>
       <c r="D5">
         <v>-2</v>
@@ -990,10 +990,10 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>-1.6</v>
+        <v>-1</v>
       </c>
       <c r="D6">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1004,10 +1004,94 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>-1.6</v>
+        <v>-1</v>
       </c>
       <c r="D7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-0.4</v>
+      </c>
+      <c r="D8">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>-0.4</v>
+      </c>
+      <c r="D9">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>-2</v>
+      </c>
+      <c r="D10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>-2</v>
+      </c>
+      <c r="D11">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-1</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to the location judgment. Planning to simplify the responses.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1_train.xlsx
+++ b/cond-files/cond_pm1_train.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\pm\pm\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B86DD2-AE48-4501-8C8E-F9E93D2EBAB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8E055E-5404-4B86-98C2-A7006D8A6063}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-144" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-144" yWindow="12855" windowWidth="23263" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>stim1_c</t>
   </si>
@@ -38,7 +38,16 @@
     <t>SOA</t>
   </si>
   <si>
-    <t>angle_diff</t>
+    <t>stim1_ori</t>
+  </si>
+  <si>
+    <t>stim2_ori</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -904,15 +913,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -920,180 +927,88 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>-0.4</v>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>-0.4</v>
+        <v>-0.8</v>
+      </c>
+      <c r="E2">
+        <v>-0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>-0.4</v>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>-0.4</v>
+        <v>-0.8</v>
+      </c>
+      <c r="E3">
+        <v>-0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>-2</v>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>-2</v>
+        <v>-0.8</v>
+      </c>
+      <c r="E4">
+        <v>-0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>-2</v>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>-2</v>
+        <v>-0.8</v>
+      </c>
+      <c r="E5">
+        <v>-0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>-1</v>
-      </c>
-      <c r="D6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>-1</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>-0.4</v>
-      </c>
-      <c r="D8">
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>-0.4</v>
-      </c>
-      <c r="D9">
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>-2</v>
-      </c>
-      <c r="D10">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>-2</v>
-      </c>
-      <c r="D11">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>-1</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>-1</v>
-      </c>
-      <c r="D13">
-        <v>-1</v>
-      </c>
-    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>